<commit_message>
Update Sentiment Analysis Models - In Depth Results.xlsx
</commit_message>
<xml_diff>
--- a/Sentiment Analysis Models - In Depth Results.xlsx
+++ b/Sentiment Analysis Models - In Depth Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e55a912db83fd400/Desktop/DissertationRepository2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clayt\OneDrive\Desktop\DissertationRepository2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="13_ncr:1_{A9A75A75-A1C4-41E4-9CF4-DBE1A6C1BAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B50A987C-5240-4C27-95AA-0A8C473D970F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3113D08D-D285-40BB-9192-D64EBB5DB1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6" xr2:uid="{A326EF4F-025B-49C9-9E5D-93C75AC21594}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A326EF4F-025B-49C9-9E5D-93C75AC21594}"/>
   </bookViews>
   <sheets>
     <sheet name="VADER" sheetId="7" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="959">
   <si>
     <t>Validation accuracy: 0.7764 with hyperparameters: {'num_filters': 128.0, 'pool_size': 4.0, 'lstm_out': 256.0, 'dropout_rate': 0.4}</t>
   </si>
@@ -4106,10 +4106,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C270D486-B562-4660-9CF3-D71B4B5BB641}" name="Table110" displayName="Table110" ref="A1:D5" totalsRowShown="0">
   <autoFilter ref="A1:D5" xr:uid="{C270D486-B562-4660-9CF3-D71B4B5BB641}"/>
@@ -4559,8 +4555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F88775-41E5-4883-ADA3-E4FA8EBD55A2}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4580,9 +4576,6 @@
       </c>
       <c r="D1" t="s">
         <v>97</v>
-      </c>
-      <c r="E1" t="s">
-        <v>937</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -9829,7 +9822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BEEFC2-1DF8-4A8F-8685-74C9C04A1756}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>